<commit_message>
Added inserts to genre and esrb tables
</commit_message>
<xml_diff>
--- a/CS+3550+-+Aggregation+Data+Set.xlsx
+++ b/CS+3550+-+Aggregation+Data+Set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03cjm\Documents\GitHub\3550GroupAssignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5B5984-DAA9-45BF-A0B7-91C84922B6DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D23B8DE-2E81-405C-828E-ECC4E86D4F94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="10596" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="10596" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregate Data Set" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
   <si>
     <t>InvoiceID</t>
   </si>
@@ -311,12 +311,6 @@
     <t>GameName</t>
   </si>
   <si>
-    <t xml:space="preserve">ESRB </t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
     <t>Missile Command</t>
   </si>
   <si>
@@ -420,6 +414,60 @@
   </si>
   <si>
     <t xml:space="preserve">Last of Us </t>
+  </si>
+  <si>
+    <t>IsOnline</t>
+  </si>
+  <si>
+    <t>ratingID</t>
+  </si>
+  <si>
+    <t>INSERT @Console (ConsoleID,ManufacturerID, ConsoleName) VALUES ('523','6','Wonder Swan')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Action')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Adventure')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Role Play')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Strategy')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Platform')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Sports')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Shooter')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Music')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Racing')</t>
+  </si>
+  <si>
+    <t>INSERT Genre(GenreName) VALUES ('Fighting')</t>
+  </si>
+  <si>
+    <t>INSERT ESRB(ESRB) VALUES ('E')</t>
+  </si>
+  <si>
+    <t>INSERT ESRB(ESRB) VALUES ('E 10+')</t>
+  </si>
+  <si>
+    <t>INSERT ESRB(ESRB) VALUES ('T')</t>
+  </si>
+  <si>
+    <t>INSERT ESRB(ESRB) VALUES ('M')</t>
+  </si>
+  <si>
+    <t>INSERT ESRB(ESRB) VALUES ('KA')</t>
   </si>
 </sst>
 </file>
@@ -16041,8 +16089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C5:V29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16441,7 +16489,7 @@
         <v>86</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="0"/>
+        <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;C28&amp;"','"&amp;D28&amp;"','"&amp;E28&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('522','2','Nintendo 64')</v>
       </c>
     </row>
@@ -16454,6 +16502,9 @@
       </c>
       <c r="E29" s="3" t="s">
         <v>87</v>
+      </c>
+      <c r="J29" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -16466,7 +16517,7 @@
   <dimension ref="C4:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16482,13 +16533,13 @@
         <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
@@ -16496,7 +16547,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -16510,7 +16564,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -16527,7 +16581,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7">
         <v>7</v>
@@ -16544,7 +16598,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -16561,7 +16615,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -16578,7 +16632,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -16595,7 +16649,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -16612,7 +16666,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E12">
         <v>9</v>
@@ -16629,7 +16683,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E13">
         <v>7</v>
@@ -16646,7 +16700,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -16663,7 +16717,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -16680,7 +16734,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -16697,7 +16751,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -16714,7 +16768,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -16731,7 +16785,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -16748,7 +16802,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -16788,60 +16842,75 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C045F4A8-5729-493B-8A8F-2CC535964053}">
-  <dimension ref="C3:D8"/>
+  <dimension ref="C3:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -16851,10 +16920,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B1CCD9-5528-4971-AF33-D6A80A4E0944}">
-  <dimension ref="C4:D14"/>
+  <dimension ref="C4:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16863,92 +16932,122 @@
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
         <v>100</v>
       </c>
-      <c r="D4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="F9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="F10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="F12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="F13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>118</v>
+      </c>
+      <c r="F14" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>